<commit_message>
Update TestCase Semi Final Sisa TestStep, karena Kode Error
</commit_message>
<xml_diff>
--- a/test_case/TestCase_Login, Create, EcosCalc.xlsx
+++ b/test_case/TestCase_Login, Create, EcosCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\Tubes\EcoSphera\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FE13A-F271-4F96-83C3-5AEC1C54BE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EABC0-93E5-41F2-A1F0-DD56D31027C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="234">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -457,12 +457,6 @@
     <t>EC12</t>
   </si>
   <si>
-    <t>EC13</t>
-  </si>
-  <si>
-    <t>EC14</t>
-  </si>
-  <si>
     <t>Create bank sampah sebagai admin</t>
   </si>
   <si>
@@ -630,15 +624,6 @@
     <t>Create bank sampah dengan  nama bank sampah mengandung angka sebagai pengelola</t>
   </si>
   <si>
-    <t>Create bank sampah dengan memasukkan harga negati untuk harga sampah organik sebagai pengelola</t>
-  </si>
-  <si>
-    <t>Create bank sampah dengan memasukkan harga negati untuk harga sampah non-organik sebagai pengelola</t>
-  </si>
-  <si>
-    <t>Create bank sampah dengan memasukkan harga negati untuk harga sampah organik dan non-organik sebagai pengelola</t>
-  </si>
-  <si>
     <t>Create bank sampah dengan data kontak lebih dari 15 digit angka sebagai peneglola</t>
   </si>
   <si>
@@ -652,6 +637,471 @@
   </si>
   <si>
     <t>Create bank sampah dengan data harga sampah non-organik lebih dari 255 karakter sebagai pengelola</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 2
+6. Ketik 1
+7. Kosongkan nama bank sampah
+8. Kosongkan nama pengelola
+9. Kosongkan Lokasi
+10. Kosongkan kontak pengelola
+11. Kosongkan harga sampah organik
+12. Kosongkan harga sampah non-organik</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 2
+6. Ketik 1
+7. Ketik 1
+8.  Kosongkan nama bank sampah
+9.  Kosongkan Lokasi
+10.  Kosongkan kontak pengelola
+11.  Kosongkanharga sampah organik
+12.  Kosongkan harga sampah non-organik</t>
+  </si>
+  <si>
+    <t>Melakukan Proses Ecoscalc dengan data numerik valid sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan Proses Ecoscalc dengan data numerik valid sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: -
+Nama Pengelola: -
+Lokasi: -
+Kontak Pengelola: -
+Harga sampah organik: -
+Harga sampah non organik: -</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa data bank sampah tidak boleh kosong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Nama bank sampah: 
+Lokasi: 
+Kontak Pengelola: 
+Harga sampah organik: 
+Harga sampah non organik: </t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: Kosong Delapan
+Harga sampah organik: 10000
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa kontak harus diisi dengan angka</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: Kosong delapan
+Harga sampah organik: 20000
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: Sepuluh
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: 10000
+Harga sampah non organik: Lima Belas Ribu</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: 08111035890
+Harga sampah organik: Dua
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: 08111035890
+Harga sampah organik: 20000
+Harga sampah non organik: Tiga Puluh Ribu</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: &lt;&gt;#$%$$^$
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: 10000
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: &lt;&gt;#$%^&amp;*
+Lokasi: Qingce Village
+Kontak Pengelola: 08111035890
+Harga sampah organik: 20000
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa harga sampah harus diisi dengan angka</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa nama bank sampah tidak mendukung simbol</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: -
+Harga sampah organik: 10000
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Muncul pemberitahuan bahwa data kontak tidak boleh kosong</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: 
+Harga sampah organik: 20000
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: -
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Muncul pemberitahuan bahwa harga sampah tidak boleh kosong</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: 10000
+Harga sampah non organik: -</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: 08111035890
+Harga sampah organik: 20000
+Harga sampah non organik: -</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Village
+Kontak Pengelola: 08111035890
+Harga sampah organik: -
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Villageeeeeeeeeeee (e x260)
+Kontak Pengelola: 08111035890
+Harga sampah organik: 20000
+Harga sampah non organik: 30000</t>
+  </si>
+  <si>
+    <t>Create bank sampah berhasil dan data tersimpan</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: a (x 256)
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: 10000
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahun Nama Bank sampah sudah ada silahkan ganti dengan nama lain</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko Centre
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890
+Harga sampah organik: 12000
+Harga sampah non organik: 13000</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890
+Harga sampah organik: 12000
+Harga sampah non organik: 13001</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890
+Harga sampah organik: 12000
+Harga sampah non organik: -13002</t>
+  </si>
+  <si>
+    <t>Muncul pemberitahuan bahwa harga sampah tidak boleh negatif</t>
+  </si>
+  <si>
+    <t>Create bank sampah dengan memasukkan harga negatif untuk harga sampah non-organik sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Create bank sampah dengan memasukkan harga negatif untuk harga sampah organik sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890
+Harga sampah organik: -12000
+Harga sampah non organik: 13003</t>
+  </si>
+  <si>
+    <t>Create bank sampah dengan memasukkan harga negatif untuk harga sampah organik dan non-organik sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890
+Harga sampah organik: -12000
+Harga sampah non organik: -13004</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: Qingce Villageee
+Kontak Pengelola: 081035890476759869486
+Harga sampah organik: 12000
+Harga sampah non organik: 13000</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: 4596464686
+Kontak Pengelola: 080102030405
+Harga sampah organik: 10000
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Muncul Peringatan Bahwa Lokasi tidak boleh diisi dengan angka</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: 74574658764
+Kontak Pengelola: 08103589047
+Harga sampah organik: 12000
+Harga sampah non organik: 13000</t>
+  </si>
+  <si>
+    <t>Username: admin
+Password: admin
+Nama bank sampah: Mondstadt Trash Bank
+Nama Pengelola: Jean
+Lokasi: Springvale
+Kontak Pengelola: 080102030405
+Harga sampah organik: 
+1000046765376498665967686436963467465476665936874685634765873644583548357453583254685348253452834582358583563546565325483458354653845238547523874582345287347345823583254623546253485234635465322376456234563254623564253487532845848753752875428532845835484582356525481835725482548725348154872538751487573451852732547235812458328751873258715423578
+Harga sampah non organik: 15000</t>
+  </si>
+  <si>
+    <t>Username: pengelola
+Password: pengelola
+Nama bank sampah: Liyue Ginko24
+Lokasi: 74574658764
+Kontak Pengelola: 08103589047
+Harga sampah organik: 12000
+Harga sampah non organik: 
+1000046765376498665967686436963467465476665936874685634765873644583548357453583254685348253452834582358583563546565325483458354653845238547523874582345287347345823583254623546253485234635465322376456234563254623564253487532845848753752875428532845835484582356525481835725482548725348154872538751487573451852732547235812458328751873258715423578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: 10
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: 10
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t>Proses EcosCalc berhasil dan menampilkan kisaran harga hasil perhitungan</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik negatif sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah non-organik negatif sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan  menginputkan berat sampah organik dengan simbol sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan  menginputkan berat sampah non-organik dengan simbol sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan Menginputkan berat kedua jenis sampah dengan simbol sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan menginputkan berat sampah organik lebih dari 255 karakter sebagai  pengelola</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan menginputkan berat sampah non-organik lebih dari 255 karakter sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan berat sampah organik kosong sebagai pengelola</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan berat sampah non-organik kosong sebagai admin</t>
+  </si>
+  <si>
+    <t>Melakukan EcosCalc dengan berat kedua jenis sampah kosong sebagai pengelola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: -10
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t>Proses EcosCalc gagal dan menampilkan pemberitahuan berat sampah tidak boleh negatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: @$%^#^#
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t>Proses EcosCalc gagal dan menampilkan pemberitahuan berat sampah tidak boleh diinput dengan simbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: 10
+Berat sampah non-organik: -10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: 10
+Berat sampah non-organik: @$%#&amp;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: @$%^#^#
+Berat sampah non-organik: @$$##
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: 1000046765376498665967686436963467465476665936874685634765873644583548357453583254685348253452834582358583563546565325483458354653845238547523874582345287347345823583254623546253485234635465322376456234563254623564253487532845848753752875428532845835484582356525481835725482548725348154872538751487573451852732547235812458328751873258715423578
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: 10
+Berat sampah non-organik: 
+1000046765376498665967686436963467465476665936874685634765873644583548357453583254685348253452834582358583563546565325483458354653845238547523874582345287347345823583254623546253485234635465322376456234563254623564253487532845848753752875428532845835484582356525481835725482548725348154872538751487573451852732547235812458328751873258715423578
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: -
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: admin
+Password: admin
+Berat sampah Organik: 10
+Berat sampah non-organik: -
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: pengelola
+Password: pengelola
+Berat sampah Organik: -
+Berat sampah non-organik: -
+</t>
+  </si>
+  <si>
+    <t>Proses EcosCalc gagal dan menampilkan pemberitahuan berat sampah tidak boleh kosong</t>
   </si>
 </sst>
 </file>
@@ -721,7 +1171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -760,6 +1210,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1748,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F2351C-0385-4866-ADB3-A4B35A9E7E31}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1800,16 +2269,16 @@
         <v>87</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -1819,381 +2288,497 @@
         <v>89</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>123</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="186" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
+        <v>122</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="186" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10"/>
+        <v>123</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>180</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>185</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>185</v>
+      </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>185</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>185</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>192</v>
+      </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>196</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10"/>
+      <c r="D27" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>196</v>
+      </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
+      <c r="D28" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>196</v>
+      </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
+      <c r="D29" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
+      <c r="D30" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="124" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="345.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10"/>
+      <c r="D32" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="295" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10"/>
+      <c r="D33" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>190</v>
+      </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
     </row>
@@ -2274,8 +2859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D4FBA-9F08-4D46-96A1-763A4AF2F165}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2283,7 +2868,7 @@
     <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" customWidth="1"/>
     <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+    <col min="4" max="4" width="50.6328125" style="4" customWidth="1"/>
     <col min="5" max="5" width="35.6328125" customWidth="1"/>
     <col min="6" max="6" width="30.6328125" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" customWidth="1"/>
@@ -2293,6 +2878,10 @@
       <c r="A1" s="13" t="s">
         <v>88</v>
       </c>
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
@@ -2317,228 +2906,296 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="C4" s="11"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>211</v>
+      </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>222</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>212</v>
+      </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>222</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="258.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>216</v>
+      </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="232.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>217</v>
+      </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>218</v>
+      </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>233</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2547,7 +3204,7 @@
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2556,7 +3213,7 @@
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="8"/>
+      <c r="D27" s="9"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -2565,7 +3222,7 @@
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="8"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -2574,7 +3231,7 @@
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="8"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -2583,7 +3240,7 @@
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="8"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -2592,7 +3249,7 @@
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="8"/>
+      <c r="D31" s="9"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
@@ -2601,7 +3258,7 @@
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="8"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -2610,7 +3267,7 @@
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="8"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -2619,7 +3276,7 @@
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="8"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
@@ -2628,7 +3285,7 @@
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="8"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
@@ -2637,7 +3294,7 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="8"/>
+      <c r="D36" s="9"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>

</xml_diff>

<commit_message>
Hasil test Pribadi LEC
</commit_message>
<xml_diff>
--- a/test_case/TestCase_Login, Create, EcosCalc.xlsx
+++ b/test_case/TestCase_Login, Create, EcosCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\Tubes\EcoSphera\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EABC0-93E5-41F2-A1F0-DD56D31027C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876449CA-BCA3-4DF5-A1A0-95B908E8FAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="253">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -168,12 +168,6 @@
   </si>
   <si>
     <t>LG07</t>
-  </si>
-  <si>
-    <t>LG08</t>
-  </si>
-  <si>
-    <t>LG09</t>
   </si>
   <si>
     <t>LG10</t>
@@ -356,23 +350,6 @@
     <t>PASS/FAIL</t>
   </si>
   <si>
-    <t>Login dengan Spasi di Username</t>
-  </si>
-  <si>
-    <t>Username: user 1
-Password: rafi 1</t>
-  </si>
-  <si>
-    <t>Login dengan Spasi di Password</t>
-  </si>
-  <si>
-    <t>Username: user1
-Password: rafi 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login Berhasil dan masuk ke menu home </t>
-  </si>
-  <si>
     <t>TestCase Create</t>
   </si>
   <si>
@@ -705,9 +682,6 @@
 Harga sampah non organik: 15000</t>
   </si>
   <si>
-    <t>Muncul Pemberitahuan bahwa kontak harus diisi dengan angka</t>
-  </si>
-  <si>
     <t>Username: pengelola
 Password: pengelola
 Nama bank sampah: Liyue Ginko Centre
@@ -863,9 +837,6 @@
 Kontak Pengelola: 080102030405
 Harga sampah organik: 10000
 Harga sampah non organik: 15000</t>
-  </si>
-  <si>
-    <t>Muncul Pemberitahun Nama Bank sampah sudah ada silahkan ganti dengan nama lain</t>
   </si>
   <si>
     <t>Username: pengelola
@@ -1102,6 +1073,110 @@
   </si>
   <si>
     <t>Proses EcosCalc gagal dan menampilkan pemberitahuan berat sampah tidak boleh kosong</t>
+  </si>
+  <si>
+    <t>Melakukan Proses Ecoscalc dengan data numerik valid sebagai user</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik negatif sebagai user</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah non-organik negatif sebagai user</t>
+  </si>
+  <si>
+    <t>EC13</t>
+  </si>
+  <si>
+    <t>EC14</t>
+  </si>
+  <si>
+    <t>EC15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: 10
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: -10
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t>Sesuai Ekspetasi</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa kontak harus diisi dengan angka minimal 7 dan maksimal 15</t>
+  </si>
+  <si>
+    <t>Tidak sesuai, data bank sampah berhasilo dibuat dengan data sampah non-organik string</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan nama Bank sampah hanya boleh berisi huruf dan minimal 3</t>
+  </si>
+  <si>
+    <t>Muncul Pemberitahuan bahwa EcosCalc hanya boleh 3 digit angka</t>
+  </si>
+  <si>
+    <t>Kode error karena belum di validasi</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>MALAH MASUK</t>
+  </si>
+  <si>
+    <t>EC16</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah non-organik 0 (nol) sebagai user</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik 0 (nol) sebagai user</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik dan non-organik 0 (nol) sebagai user</t>
+  </si>
+  <si>
+    <t>EC17</t>
+  </si>
+  <si>
+    <t>EC18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: 10
+Berat sampah non-organik: 0
+</t>
+  </si>
+  <si>
+    <t>Proses EcosCalc gagal dan menampilkan pemberitahuan berat sampah tidak boleh nol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: 0
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: 0
+Berat sampah non-organik: 0
+</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1210,24 +1285,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1663,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB37F0-9CC2-46A0-A4C5-898826E3FD91}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1678,20 +1741,21 @@
     <col min="5" max="5" width="35.6328125" customWidth="1"/>
     <col min="6" max="6" width="30.6328125" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="12" max="13" width="30.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1</v>
@@ -1709,276 +1773,346 @@
         <v>5</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L4" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L5" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L6" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L7" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L8" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L9" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L10" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L12" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L13" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="L14" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="186" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="186" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="L15" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -1987,7 +2121,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -1996,7 +2130,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -2005,7 +2139,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -2014,7 +2148,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
@@ -2023,7 +2157,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -2032,7 +2166,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
@@ -2041,7 +2175,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -2050,7 +2184,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -2059,7 +2193,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -2068,7 +2202,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -2077,7 +2211,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -2086,7 +2220,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -2095,7 +2229,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -2104,7 +2238,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
@@ -2215,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F2351C-0385-4866-ADB3-A4B35A9E7E31}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2230,20 +2364,21 @@
     <col min="5" max="5" width="35.6328125" customWidth="1"/>
     <col min="6" max="6" width="30.6328125" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="12" max="13" width="30.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1</v>
@@ -2261,570 +2396,756 @@
         <v>5</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="186" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="B4" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="186" x14ac:dyDescent="0.35">
+      <c r="L4" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="186" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="186" x14ac:dyDescent="0.35">
+      <c r="L5" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="186" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="186" x14ac:dyDescent="0.35">
+      <c r="L6" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="186" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L7" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L8" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L9" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L10" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L12" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L13" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L14" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L15" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L16" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L17" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L18" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L19" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L20" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L21" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L22" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L23" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L24" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L25" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L26" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L27" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L28" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="1:7" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="L29" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="L30" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="124" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" ht="345.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L31" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M31" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="345.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" ht="295" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L32" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="295" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L33" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M33" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.35">
@@ -2857,10 +3178,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D4FBA-9F08-4D46-96A1-763A4AF2F165}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2872,20 +3193,21 @@
     <col min="5" max="5" width="35.6328125" customWidth="1"/>
     <col min="6" max="6" width="30.6328125" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="12" max="13" width="30.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1</v>
@@ -2903,295 +3225,456 @@
         <v>5</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L4" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L5" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L6" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L7" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" s="17"/>
+        <v>204</v>
+      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C9" s="17"/>
+        <v>205</v>
+      </c>
+      <c r="C9" s="11"/>
       <c r="D9" s="11" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" ht="258.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="L10" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="258.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="232.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="232.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L12" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="L13" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="93" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C14" s="17"/>
+        <v>210</v>
+      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="L14" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="L15" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="93" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="11" t="s">
+      <c r="E16" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="L16" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="L17" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E18" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="L18" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="L19" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="L20" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="L21" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -3200,7 +3683,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -3209,7 +3692,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -3218,7 +3701,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -3227,7 +3710,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -3236,7 +3719,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -3245,7 +3728,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -3254,7 +3737,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>

</xml_diff>

<commit_message>
Final, Sudah ada steps plus tambahan file dari hasil cek pribadi
</commit_message>
<xml_diff>
--- a/test_case/TestCase_Login, Create, EcosCalc.xlsx
+++ b/test_case/TestCase_Login, Create, EcosCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\Tubes\EcoSphera\test_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876449CA-BCA3-4DF5-A1A0-95B908E8FAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E001EDF8-B556-4DCA-BC35-16570FCA9473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7517725E-8658-40C2-8654-0FE0DDC87835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="264">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1107,34 +1107,13 @@
 </t>
   </si>
   <si>
-    <t>Sesuai Ekspetasi</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Muncul Pemberitahuan bahwa kontak harus diisi dengan angka minimal 7 dan maksimal 15</t>
   </si>
   <si>
-    <t>Tidak sesuai, data bank sampah berhasilo dibuat dengan data sampah non-organik string</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Muncul Pemberitahuan nama Bank sampah hanya boleh berisi huruf dan minimal 3</t>
   </si>
   <si>
     <t>Muncul Pemberitahuan bahwa EcosCalc hanya boleh 3 digit angka</t>
-  </si>
-  <si>
-    <t>Kode error karena belum di validasi</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>MALAH MASUK</t>
   </si>
   <si>
     <t>EC16</t>
@@ -1177,6 +1156,141 @@
 Berat sampah Organik: 0
 Berat sampah non-organik: 0
 </t>
+  </si>
+  <si>
+    <t>Create bank sampah sebagai pengelola yang belum memiliki bank sampah</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>Username: LyoidHyper01
+Password: IamSpy01
+Nama bank sampah: Forgers Bank
+Lokasi: Kadipaten Brundhilde
+Kontak Pengelola: 0887987654
+Harga sampah organik: 10000
+Harga sampah non organik: 10000</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 1
+6. Pilih Bank Sampah (Ketik 0)
+7. Masukkan berat sampah organik
+8. Masukkan Berat sampah non-organik
+9. Enter
+10. Ketik 2
+11. Enter
+12. Ketik 6
+13. Enter</t>
+  </si>
+  <si>
+    <t>EC19</t>
+  </si>
+  <si>
+    <t>EC20</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik dan non-organik kosong sebagai user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: -
+Berat sampah non-organik: -
+</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah organik  kosong sebagai user</t>
+  </si>
+  <si>
+    <t>Melakukan proses EcosCalc dengan data berat sampah non-organik kosong sebagai user</t>
+  </si>
+  <si>
+    <t>EC21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: -
+Berat sampah non-organik: 10
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: user
+Password: user
+Berat sampah Organik: 10
+Berat sampah non-organik: -
+</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 2
+6. Ketik 1
+7. Masukkan nama bank sampah
+8. Masukkan Lokasi
+9. Masukkan kontak pengelola
+10. Masukkan harga sampah organik
+11. Masukkan harga sampah non-organik
+12. Enter</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 1
+6. Pilih Bank Sampah (Ketik 0)
+7. Masukkan berat sampah organik
+8. Masukkan Berat sampah non-organik
+9. Enter
+10. Ketik q
+11. Enter</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 1
+6. Pilih Bank Sampah (Ketik 0)
+7. Kosongkan berat sampah organik
+8. Masukkan Berat sampah non-organik
+9. Enter
+10. Ketik q
+11. Enter</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 1
+6. Pilih Bank Sampah (Ketik 0)
+7. Masukkan berat sampah organik
+8. Kosongkan Berat sampah non-organik
+9. Enter
+10. Ketik q
+11. Enter</t>
+  </si>
+  <si>
+    <t>1. Jalankan program
+2. Ketik 2
+3. Masukkan Username
+4. Masukkan Password
+5. Ketik 1
+6. Pilih Bank Sampah (Ketik 0)
+7. Kosongkan berat sampah organik
+8. Kosongkan Berat sampah non-organik
+9. Enter
+10. Ketik q
+11. Enter</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1285,13 +1399,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,17 +1724,17 @@
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.54296875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1673,7 +1780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1696,7 +1803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1728,32 +1835,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BB37F0-9CC2-46A0-A4C5-898826E3FD91}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.6328125" customWidth="1"/>
-    <col min="6" max="6" width="30.6328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="12" max="13" width="30.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="12" max="13" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>77</v>
       </c>
@@ -1775,14 +1882,8 @@
       <c r="G3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
@@ -1800,14 +1901,8 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="L4" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
@@ -1825,14 +1920,8 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="L5" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
@@ -1850,14 +1939,8 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="L6" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
@@ -1875,14 +1958,8 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="L7" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>32</v>
       </c>
@@ -1900,14 +1977,8 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="L8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>33</v>
       </c>
@@ -1925,14 +1996,8 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
@@ -1950,14 +2015,8 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="L10" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:13" ht="126" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
@@ -1975,14 +2034,8 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
@@ -2000,14 +2053,8 @@
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="L12" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
@@ -2025,14 +2072,8 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="L13" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="77.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>59</v>
       </c>
@@ -2050,14 +2091,8 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="L14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:13" ht="189" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>60</v>
       </c>
@@ -2075,44 +2110,20 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="L15" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -2121,7 +2132,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -2130,7 +2141,7 @@
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -2139,7 +2150,7 @@
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -2148,7 +2159,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
@@ -2157,7 +2168,7 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -2166,7 +2177,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
@@ -2175,7 +2186,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -2184,7 +2195,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -2193,7 +2204,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -2202,7 +2213,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -2211,7 +2222,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -2220,7 +2231,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -2229,7 +2240,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -2238,7 +2249,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
@@ -2247,7 +2258,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
@@ -2256,7 +2267,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
@@ -2265,7 +2276,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
@@ -2274,7 +2285,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
@@ -2283,61 +2294,61 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
     </row>
   </sheetData>
@@ -2349,34 +2360,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F2351C-0385-4866-ADB3-A4B35A9E7E31}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="45.6328125" customWidth="1"/>
-    <col min="4" max="4" width="45.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.6328125" customWidth="1"/>
-    <col min="6" max="6" width="30.6328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="12" max="13" width="30.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="12" max="13" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>79</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>77</v>
       </c>
@@ -2398,14 +2409,8 @@
       <c r="G3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>80</v>
       </c>
@@ -2423,14 +2428,8 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="L4" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>82</v>
       </c>
@@ -2448,14 +2447,8 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="L5" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
@@ -2473,14 +2466,8 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="L6" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="186" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -2498,67 +2485,55 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="L7" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D8" s="11" t="s">
         <v>163</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="L8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D9" s="11" t="s">
         <v>164</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D10" s="11" t="s">
         <v>165</v>
       </c>
@@ -2567,21 +2542,17 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="L10" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D11" s="11" t="s">
         <v>167</v>
       </c>
@@ -2590,21 +2561,17 @@
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D12" s="11" t="s">
         <v>166</v>
       </c>
@@ -2613,21 +2580,17 @@
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="L12" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D13" s="11" t="s">
         <v>168</v>
       </c>
@@ -2636,21 +2599,17 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="L13" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D14" s="11" t="s">
         <v>169</v>
       </c>
@@ -2659,21 +2618,17 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="L14" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D15" s="11" t="s">
         <v>170</v>
       </c>
@@ -2682,21 +2637,17 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="L15" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D16" s="11" t="s">
         <v>173</v>
       </c>
@@ -2705,21 +2656,17 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="L16" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>94</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>175</v>
       </c>
@@ -2728,21 +2675,17 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="L17" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D18" s="11" t="s">
         <v>176</v>
       </c>
@@ -2751,21 +2694,17 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="L18" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>125</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D19" s="11" t="s">
         <v>180</v>
       </c>
@@ -2774,21 +2713,17 @@
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="L19" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>126</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D20" s="11" t="s">
         <v>178</v>
       </c>
@@ -2797,21 +2732,17 @@
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="L20" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D21" s="11" t="s">
         <v>179</v>
       </c>
@@ -2820,21 +2751,17 @@
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="L21" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>128</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D22" s="11" t="s">
         <v>181</v>
       </c>
@@ -2843,21 +2770,17 @@
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="L22" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D23" s="11" t="s">
         <v>183</v>
       </c>
@@ -2866,21 +2789,17 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="L23" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>130</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D24" s="11" t="s">
         <v>184</v>
       </c>
@@ -2889,44 +2808,36 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="L24" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M24" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>131</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D25" s="11" t="s">
         <v>185</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="L25" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M25" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>132</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D26" s="11" t="s">
         <v>186</v>
       </c>
@@ -2935,21 +2846,17 @@
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="L26" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M26" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>133</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D27" s="11" t="s">
         <v>190</v>
       </c>
@@ -2958,21 +2865,17 @@
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="L27" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>134</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D28" s="11" t="s">
         <v>192</v>
       </c>
@@ -2981,44 +2884,36 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="L28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D29" s="11" t="s">
         <v>193</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="L29" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M29" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="139.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>136</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D30" s="11" t="s">
         <v>194</v>
       </c>
@@ -3027,21 +2922,17 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="L30" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="124" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:7" ht="189" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>137</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D31" s="11" t="s">
         <v>196</v>
       </c>
@@ -3050,21 +2941,17 @@
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="L31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M31" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="345.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:7" ht="345.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>138</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D32" s="11" t="s">
         <v>197</v>
       </c>
@@ -3073,21 +2960,17 @@
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="L32" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="295" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:7" ht="294.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>139</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="D33" s="11" t="s">
         <v>198</v>
       </c>
@@ -3096,77 +2979,87 @@
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="L33" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M33" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:7" ht="189" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
     </row>
   </sheetData>
@@ -3178,34 +3071,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D4FBA-9F08-4D46-96A1-763A4AF2F165}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="50.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.6328125" customWidth="1"/>
-    <col min="6" max="6" width="30.6328125" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
-    <col min="12" max="13" width="30.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="12" max="13" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>81</v>
       </c>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>77</v>
       </c>
@@ -3227,21 +3120,17 @@
       <c r="G3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="D4" s="11" t="s">
         <v>199</v>
       </c>
@@ -3250,21 +3139,17 @@
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="L4" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="D5" s="11" t="s">
         <v>200</v>
       </c>
@@ -3273,21 +3158,17 @@
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="L5" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D6" s="11" t="s">
         <v>212</v>
       </c>
@@ -3296,21 +3177,17 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="L6" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D7" s="11" t="s">
         <v>216</v>
       </c>
@@ -3319,21 +3196,17 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="L7" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D8" s="11" t="s">
         <v>214</v>
       </c>
@@ -3342,21 +3215,17 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="L8" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D9" s="11" t="s">
         <v>217</v>
       </c>
@@ -3365,21 +3234,17 @@
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D10" s="11" t="s">
         <v>218</v>
       </c>
@@ -3388,67 +3253,55 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="L10" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="258.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" ht="258.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D11" s="11" t="s">
         <v>219</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="L11" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="232.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" ht="232.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D12" s="11" t="s">
         <v>220</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="L12" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="11" t="s">
+        <v>261</v>
+      </c>
       <c r="D13" s="11" t="s">
         <v>221</v>
       </c>
@@ -3457,21 +3310,17 @@
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="L13" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="D14" s="11" t="s">
         <v>222</v>
       </c>
@@ -3480,21 +3329,17 @@
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="L14" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>263</v>
+      </c>
       <c r="D15" s="11" t="s">
         <v>223</v>
       </c>
@@ -3503,21 +3348,17 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="L15" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>228</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="D16" s="11" t="s">
         <v>231</v>
       </c>
@@ -3526,21 +3367,17 @@
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="L16" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>229</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>231</v>
       </c>
@@ -3549,21 +3386,17 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="L17" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>230</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D18" s="11" t="s">
         <v>232</v>
       </c>
@@ -3572,109 +3405,122 @@
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="L18" s="10" t="s">
+    </row>
+    <row r="19" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="M18" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="93" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>250</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="L19" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="11"/>
+        <v>238</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D20" s="11" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="L20" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="93" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C21" s="11"/>
+        <v>239</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="D21" s="11" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="L21" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -3683,7 +3529,7 @@
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -3692,7 +3538,7 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -3701,7 +3547,7 @@
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -3710,7 +3556,7 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -3719,7 +3565,7 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
@@ -3728,7 +3574,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -3737,7 +3583,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
@@ -3746,7 +3592,7 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="9"/>
@@ -3755,7 +3601,7 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="9"/>
@@ -3764,7 +3610,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="9"/>
@@ -3773,7 +3619,7 @@
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
@@ -3782,61 +3628,61 @@
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
     </row>
   </sheetData>

</xml_diff>